<commit_message>
Added packet information captured by wireshark to Sightline folder.
</commit_message>
<xml_diff>
--- a/Sightline/Sightline tracking 001.xlsx
+++ b/Sightline/Sightline tracking 001.xlsx
@@ -85,6 +85,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>http://youtu.be/rMnI86wqPlU</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000" b="1" u="none"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1932,33 +1951,81 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="69815296"/>
-        <c:axId val="69825280"/>
+        <c:axId val="47753472"/>
+        <c:axId val="47755264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69815296"/>
+        <c:axId val="47753472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Data Point</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69825280"/>
+        <c:crossAx val="47755264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69825280"/>
+        <c:axId val="47755264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Pixel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> Position (out of 480)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.7830689172377872E-3"/>
+              <c:y val="0.2959529836097527"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69815296"/>
+        <c:crossAx val="47753472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1969,9 +2036,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3277072513224456"/>
-          <c:y val="4.2249293720857388E-2"/>
-          <c:w val="0.52475909090856709"/>
+          <c:x val="0.4550617506223934"/>
+          <c:y val="9.869131026268553E-2"/>
+          <c:w val="0.52475909090856721"/>
           <c:h val="0.10213846356767828"/>
         </c:manualLayout>
       </c:layout>

</xml_diff>